<commit_message>
ALPHA - Main GUI operational
</commit_message>
<xml_diff>
--- a/NTDS_Enschede.xlsx
+++ b/NTDS_Enschede.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="18000" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="18600" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1159,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W74"/>
+  <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4514,34 +4514,52 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="T74" s="2"/>
+      <c r="U74" s="2"/>
+      <c r="V74" s="2"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>73</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H74" t="s">
-        <v>254</v>
-      </c>
-      <c r="I74" t="s">
-        <v>254</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="K74" s="3" t="s">
+      <c r="H75" t="s">
+        <v>254</v>
+      </c>
+      <c r="I75" t="s">
+        <v>254</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="K75" s="3" t="s">
         <v>252</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ALPHA - Participating teams in config
</commit_message>
<xml_diff>
--- a/NTDS_Enschede.xlsx
+++ b/NTDS_Enschede.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="18600" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="19800" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:W75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ALPHA - Bug fixes + minor refactoring
</commit_message>
<xml_diff>
--- a/NTDS_Enschede.xlsx
+++ b/NTDS_Enschede.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20400" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="21600" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="259">
   <si>
     <t>Femke</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Keith</t>
   </si>
   <si>
-    <t>Nummer</t>
-  </si>
-  <si>
     <t>E-mail</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>Latin niveau</t>
   </si>
   <si>
-    <t>Partner Ballroom</t>
-  </si>
-  <si>
-    <t>Partner Latin</t>
-  </si>
-  <si>
     <t>Ballroom verplicht blind daten</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>Slaapplek</t>
   </si>
   <si>
-    <t>Allergiën/dieet</t>
-  </si>
-  <si>
     <t>Voornaam</t>
   </si>
   <si>
@@ -116,18 +104,6 @@
     <t>BHV</t>
   </si>
   <si>
-    <t>Jury ballroom</t>
-  </si>
-  <si>
-    <t>Jury latin</t>
-  </si>
-  <si>
-    <t>Nu vrijwilliger</t>
-  </si>
-  <si>
-    <t>Eerder vrijwilliger geweest</t>
-  </si>
-  <si>
     <t>Pepijn</t>
   </si>
   <si>
@@ -798,6 +774,33 @@
   </si>
   <si>
     <t>Beginners</t>
+  </si>
+  <si>
+    <t>Nr. Ballroom partner</t>
+  </si>
+  <si>
+    <t>Nr. Latin partner</t>
+  </si>
+  <si>
+    <t>Jury Ballroom</t>
+  </si>
+  <si>
+    <t>Jury Latin</t>
+  </si>
+  <si>
+    <t>Allergiën / dieet</t>
+  </si>
+  <si>
+    <t>Wil je vrijwilliger zijn voor dit NTDS?</t>
+  </si>
+  <si>
+    <t>Ben je op een eerder ETDS of NTDS vrijwilliger geweest?</t>
+  </si>
+  <si>
+    <t>Doe je mee aan de Same Seks wedstrijd?</t>
+  </si>
+  <si>
+    <t>Nr.</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W75"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,144 +1197,147 @@
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>31</v>
+        <v>253</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>23</v>
+        <v>254</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>32</v>
+        <v>255</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L2" s="2"/>
       <c r="O2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="S2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H3" s="2">
         <v>6</v>
@@ -1340,24 +1346,24 @@
         <v>6</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L3" s="2"/>
       <c r="O3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="S3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1365,111 +1371,111 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="S4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2">
         <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="2"/>
       <c r="O5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="S5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H6" s="2">
         <v>45</v>
@@ -1478,42 +1484,42 @@
         <v>45</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L6" s="2"/>
       <c r="O6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="S6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H7" s="2">
         <v>2</v>
@@ -1522,42 +1528,42 @@
         <v>2</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L7" s="2"/>
       <c r="O7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="S7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H8" s="2">
         <v>14</v>
@@ -1566,42 +1572,42 @@
         <v>14</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="S8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H9" s="2">
         <v>13</v>
@@ -1610,42 +1616,42 @@
         <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L9" s="2"/>
       <c r="O9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="S9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H10" s="2">
         <v>53</v>
@@ -1654,85 +1660,85 @@
         <v>53</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L10" s="2"/>
       <c r="O10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="S10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H12" s="2">
         <v>17</v>
@@ -1741,42 +1747,42 @@
         <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L12" s="2"/>
       <c r="O12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="S12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H13" s="2">
         <v>23</v>
@@ -1785,42 +1791,42 @@
         <v>23</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L13" s="2"/>
       <c r="O13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="S13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H14" s="2">
         <v>8</v>
@@ -1829,42 +1835,42 @@
         <v>8</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L14" s="2"/>
       <c r="O14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="S14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H15" s="2">
         <v>7</v>
@@ -1873,44 +1879,44 @@
         <v>7</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L15" s="2"/>
       <c r="O15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="S15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H16" s="2">
         <v>32</v>
@@ -1919,22 +1925,22 @@
         <v>32</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L16" s="2"/>
       <c r="O16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="S16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="V16" s="2"/>
     </row>
@@ -1943,47 +1949,47 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L17" s="2"/>
       <c r="O17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="S17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -1991,20 +1997,20 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H18" s="2">
         <v>11</v>
@@ -2013,22 +2019,22 @@
         <v>11</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L18" s="2"/>
       <c r="O18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="S18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="V18" s="2"/>
     </row>
@@ -2037,50 +2043,50 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="S19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
@@ -2090,41 +2096,41 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L20" s="2"/>
       <c r="O20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="S20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
@@ -2134,20 +2140,20 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H21" s="2">
         <v>27</v>
@@ -2156,22 +2162,22 @@
         <v>27</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L21" s="2"/>
       <c r="O21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="S21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="V21" s="2"/>
     </row>
@@ -2180,41 +2186,41 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L22" s="2"/>
       <c r="O22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="S22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
@@ -2224,45 +2230,45 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L23" s="2"/>
       <c r="O23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="S23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U23" s="2"/>
       <c r="V23" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -2270,20 +2276,20 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H24" s="2">
         <v>12</v>
@@ -2292,23 +2298,23 @@
         <v>12</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L24" s="2"/>
       <c r="O24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="S24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U24" s="2"/>
       <c r="V24" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2316,43 +2322,43 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="2"/>
       <c r="O25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="S25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -2360,41 +2366,41 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L26" s="2"/>
       <c r="O26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="S26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
@@ -2404,40 +2410,40 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="T27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U27" s="2"/>
       <c r="V27" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -2445,20 +2451,20 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H28" s="2">
         <v>20</v>
@@ -2467,19 +2473,19 @@
         <v>20</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L28" s="2"/>
       <c r="O28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="S28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
@@ -2489,41 +2495,41 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L29" s="2"/>
       <c r="O29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="S29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
@@ -2533,41 +2539,41 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L30" s="2"/>
       <c r="O30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="S30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
@@ -2577,38 +2583,38 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L31" s="2"/>
       <c r="O31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="S31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
@@ -2619,41 +2625,41 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L32" s="2"/>
       <c r="O32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="S32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
@@ -2663,20 +2669,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H33" s="2">
         <v>15</v>
@@ -2685,16 +2691,16 @@
         <v>15</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L33" s="2"/>
       <c r="O33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="S33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
@@ -2705,20 +2711,20 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H34" s="2">
         <v>39</v>
@@ -2727,19 +2733,19 @@
         <v>39</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L34" s="2"/>
       <c r="O34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="S34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
@@ -2749,20 +2755,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H35" s="2">
         <v>37</v>
@@ -2771,19 +2777,19 @@
         <v>37</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L35" s="2"/>
       <c r="O35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="S35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T35" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
@@ -2793,45 +2799,45 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L36" s="2"/>
       <c r="O36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="S36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U36" s="2"/>
       <c r="V36" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -2839,46 +2845,46 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="S37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T37" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
@@ -2892,16 +2898,16 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H38" s="2">
         <v>34</v>
@@ -2910,21 +2916,21 @@
         <v>34</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L38" s="2"/>
       <c r="O38" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="S38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
@@ -2938,42 +2944,42 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="S39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
@@ -2983,22 +2989,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H40" s="2">
         <v>33</v>
@@ -3007,19 +3013,19 @@
         <v>33</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L40" s="2"/>
       <c r="O40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="S40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
@@ -3029,41 +3035,41 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L41" s="2"/>
       <c r="O41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="S41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
@@ -3073,44 +3079,44 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L42" s="2"/>
       <c r="O42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="S42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="V42" s="2"/>
     </row>
@@ -3119,41 +3125,41 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L43" s="2"/>
       <c r="O43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="S43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
@@ -3163,49 +3169,49 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="S44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="V44" s="2"/>
     </row>
@@ -3214,20 +3220,20 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H45" s="2">
         <v>61</v>
@@ -3236,19 +3242,19 @@
         <v>65</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L45" s="2"/>
       <c r="O45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="S45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
@@ -3258,20 +3264,20 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H46" s="2">
         <v>5</v>
@@ -3280,19 +3286,19 @@
         <v>5</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L46" s="2"/>
       <c r="O46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="S46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
@@ -3306,42 +3312,42 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="T47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="V47" s="2"/>
     </row>
@@ -3350,43 +3356,43 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L48" s="2"/>
       <c r="O48" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="S48" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T48" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
@@ -3396,20 +3402,20 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H49" s="2">
         <v>56</v>
@@ -3418,19 +3424,19 @@
         <v>56</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L49" s="2"/>
       <c r="O49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="S49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
@@ -3440,45 +3446,45 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H50" s="2">
         <v>4</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L50" s="2"/>
       <c r="O50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="S50" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T50" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U50" s="2"/>
       <c r="V50" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
@@ -3486,42 +3492,42 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L51" s="2"/>
       <c r="O51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="S51" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T51" s="2"/>
       <c r="U51" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="V51" s="2"/>
     </row>
@@ -3530,20 +3536,20 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H52" s="2">
         <v>59</v>
@@ -3552,23 +3558,23 @@
         <v>59</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L52" s="2"/>
       <c r="O52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="S52" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T52" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U52" s="2"/>
       <c r="V52" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
@@ -3580,16 +3586,16 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H53" s="2">
         <v>64</v>
@@ -3598,26 +3604,26 @@
         <v>64</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L53" s="2"/>
       <c r="N53" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="S53" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T53" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U53" s="2"/>
       <c r="V53" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
@@ -3625,20 +3631,20 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H54" s="2">
         <v>9</v>
@@ -3647,23 +3653,23 @@
         <v>9</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L54" s="2"/>
       <c r="O54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="S54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U54" s="2"/>
       <c r="V54" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
@@ -3671,41 +3677,41 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L55" s="2"/>
       <c r="O55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="S55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
@@ -3715,45 +3721,45 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L56" s="2"/>
       <c r="O56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="S56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U56" s="2"/>
       <c r="V56" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
@@ -3761,22 +3767,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H57" s="2">
         <v>48</v>
@@ -3785,25 +3791,25 @@
         <v>48</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L57" s="2"/>
       <c r="O57" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q57" s="2"/>
       <c r="S57" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T57" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U57" s="2"/>
       <c r="V57" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
@@ -3811,22 +3817,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H58" s="2">
         <v>60</v>
@@ -3835,20 +3841,20 @@
         <v>60</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L58" s="2"/>
       <c r="O58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="S58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T58" s="2"/>
       <c r="U58" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="V58" s="2"/>
     </row>
@@ -3857,20 +3863,20 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H59" s="2">
         <v>62</v>
@@ -3879,20 +3885,20 @@
         <v>62</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L59" s="2"/>
       <c r="O59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="S59" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T59" s="2"/>
       <c r="U59" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="V59" s="2"/>
     </row>
@@ -3901,20 +3907,20 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H60" s="2">
         <v>51</v>
@@ -3923,22 +3929,22 @@
         <v>51</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L60" s="2"/>
       <c r="O60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="S60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U60" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="V60" s="2"/>
     </row>
@@ -3947,20 +3953,20 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H61" s="2">
         <v>57</v>
@@ -3969,19 +3975,19 @@
         <v>57</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L61" s="2"/>
       <c r="O61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="S61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
@@ -3991,47 +3997,47 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H62" s="2">
         <v>44</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L62" s="2"/>
       <c r="O62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="S62" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T62" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U62" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="V62" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
@@ -4039,20 +4045,20 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H63" s="2">
         <v>58</v>
@@ -4061,19 +4067,19 @@
         <v>58</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L63" s="2"/>
       <c r="O63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="S63" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T63" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
@@ -4083,20 +4089,20 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H64" s="2">
         <v>67</v>
@@ -4105,19 +4111,19 @@
         <v>67</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L64" s="2"/>
       <c r="O64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="S64" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T64" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
@@ -4131,16 +4137,16 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H65" s="2">
         <v>52</v>
@@ -4149,25 +4155,25 @@
         <v>52</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L65" s="2"/>
       <c r="O65" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="S65" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T65" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U65" s="2"/>
       <c r="V65" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
@@ -4175,43 +4181,43 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I66" s="3">
         <v>44</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L66" s="2"/>
       <c r="O66" s="2"/>
       <c r="Q66" s="2"/>
       <c r="S66" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T66" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
@@ -4221,20 +4227,20 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H67" s="2">
         <v>69</v>
@@ -4243,19 +4249,19 @@
         <v>69</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L67" s="2"/>
       <c r="O67" s="2"/>
       <c r="Q67" s="2"/>
       <c r="S67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
@@ -4265,20 +4271,20 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H68" s="2">
         <v>63</v>
@@ -4287,19 +4293,19 @@
         <v>63</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L68" s="2"/>
       <c r="O68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="S68" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T68" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
@@ -4309,41 +4315,41 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L69" s="2"/>
       <c r="O69" s="2"/>
       <c r="Q69" s="2"/>
       <c r="S69" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T69" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
@@ -4353,20 +4359,20 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H70" s="2">
         <v>66</v>
@@ -4375,19 +4381,19 @@
         <v>66</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L70" s="2"/>
       <c r="O70" s="2"/>
       <c r="Q70" s="2"/>
       <c r="S70" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T70" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
@@ -4397,42 +4403,42 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K71" s="3"/>
       <c r="L71" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O71" s="2"/>
       <c r="Q71" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T71" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U71" s="2"/>
       <c r="V71" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
@@ -4440,38 +4446,38 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="L72" s="2"/>
       <c r="O72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="T72" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
@@ -4481,88 +4487,70 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E73" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K73" s="3"/>
       <c r="L73" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
       <c r="V73" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="2"/>
-      <c r="O74" s="2"/>
-      <c r="Q74" s="2"/>
-      <c r="T74" s="2"/>
-      <c r="U74" s="2"/>
-      <c r="V74" s="2"/>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>73</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="H75" t="s">
-        <v>252</v>
-      </c>
-      <c r="I75" t="s">
-        <v>252</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>250</v>
+      <c r="G74" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H74" t="s">
+        <v>244</v>
+      </c>
+      <c r="I74" t="s">
+        <v>244</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beta 0.9 - Added selectr
</commit_message>
<xml_diff>
--- a/NTDS_Enschede.xlsx
+++ b/NTDS_Enschede.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alen\PycharmProjects\NTDS_Loting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alen\PycharmProjects\NTDS_Loting\test_signup\Amsterdam\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="21600" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="22200" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1165,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X74"/>
+  <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X1"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4522,34 +4522,52 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="T74" s="2"/>
+      <c r="U74" s="2"/>
+      <c r="V74" s="2"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>73</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="H74" t="s">
-        <v>244</v>
-      </c>
-      <c r="I74" t="s">
-        <v>244</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K74" s="3" t="s">
+      <c r="H75" t="s">
+        <v>244</v>
+      </c>
+      <c r="I75" t="s">
+        <v>244</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="K75" s="3" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>